<commit_message>
corrected false positives for "as soon as" and "as long as"
</commit_message>
<xml_diff>
--- a/UserTestEval/Data/TemplateComparison_calculatedMetricsUsertest.xlsx
+++ b/UserTestEval/Data/TemplateComparison_calculatedMetricsUsertest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\Evaluation-of-templates-for-requirements-documentation\UserTestEval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C3E973-86F0-48F3-B1F8-F0198038D2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA17A1-A212-4C1B-ABAE-5547583AD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="2625" windowWidth="25440" windowHeight="15270" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student free" sheetId="1" r:id="rId1"/>
@@ -982,9 +982,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1173,67 +1173,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1249,9 +1249,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5656,142 +5656,142 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5805,11 +5805,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5871,7 +5873,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5936,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5998,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6060,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6122,7 +6124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -6184,7 +6186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6246,7 +6248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6308,7 +6310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6370,7 +6372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6432,7 +6434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6494,7 +6496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6556,7 +6558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6579,7 +6581,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -6618,7 +6620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6680,7 +6682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6742,7 +6744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6804,7 +6806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6866,7 +6868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6928,7 +6930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6990,7 +6992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -7052,7 +7054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -7114,7 +7116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7238,7 +7240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7300,7 +7302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7362,7 +7364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -7424,7 +7426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -7486,7 +7488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -7548,7 +7550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -7610,7 +7612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -7672,7 +7674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -7695,7 +7697,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -7734,7 +7736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -7796,7 +7798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -7858,7 +7860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -7920,7 +7922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -7982,7 +7984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8044,7 +8046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -8106,7 +8108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -8168,7 +8170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -8230,7 +8232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -8253,7 +8255,7 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -8292,7 +8294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -8315,7 +8317,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -8354,7 +8356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -8377,7 +8379,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -8416,7 +8418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -8478,7 +8480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -8540,7 +8542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -8602,7 +8604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -8625,7 +8627,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -8664,7 +8666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -8726,7 +8728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -8749,7 +8751,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -8788,7 +8790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -8850,7 +8852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -8912,7 +8914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -8974,7 +8976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -9036,7 +9038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -9098,7 +9100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -9160,7 +9162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -9183,7 +9185,7 @@
         <v>1</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55">
         <v>1</v>
@@ -9222,7 +9224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -9284,7 +9286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -9307,7 +9309,7 @@
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -9346,7 +9348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -9408,7 +9410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -9470,7 +9472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -9532,7 +9534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -9594,7 +9596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -9617,7 +9619,7 @@
         <v>1</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -9656,7 +9658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -9718,7 +9720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -9780,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -9842,7 +9844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -9865,7 +9867,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -9904,7 +9906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -9927,7 +9929,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -9966,7 +9968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -10028,7 +10030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -10051,7 +10053,7 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -10090,7 +10092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -10113,7 +10115,7 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70">
         <v>1</v>
@@ -10152,7 +10154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -10175,7 +10177,7 @@
         <v>1</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -10214,7 +10216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -10276,7 +10278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -10338,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -10400,7 +10402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -10462,207 +10464,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -10678,9 +10680,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10742,7 +10744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -10807,7 +10809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10869,487 +10871,487 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -11363,11 +11365,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11429,7 +11433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -11494,7 +11498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11556,7 +11560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -11618,7 +11622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -11680,7 +11684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -11742,7 +11746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -11804,7 +11808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -11866,7 +11870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -11928,447 +11932,447 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -12382,16 +12386,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12453,7 +12457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -12518,7 +12522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -12580,7 +12584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -12642,7 +12646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -12704,7 +12708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -12766,7 +12770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -12789,7 +12793,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -12828,7 +12832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -12890,7 +12894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -12952,532 +12956,532 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -13491,11 +13495,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="19.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13557,7 +13566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -13622,7 +13631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -13684,7 +13693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -13746,7 +13755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -13808,7 +13817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -13831,7 +13840,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -13870,7 +13879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -13932,7 +13941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -13994,7 +14003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -14056,7 +14065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -14118,7 +14127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -14141,7 +14150,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -14180,7 +14189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -14242,7 +14251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -14304,512 +14313,512 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
applied extended vague term detection
</commit_message>
<xml_diff>
--- a/UserTestEval/Data/TemplateComparison_calculatedMetricsUsertest.xlsx
+++ b/UserTestEval/Data/TemplateComparison_calculatedMetricsUsertest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\Evaluation-of-templates-for-requirements-documentation\UserTestEval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA17A1-A212-4C1B-ABAE-5547583AD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FD3DB7-3628-4447-A3CB-6686F232514C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student free" sheetId="1" r:id="rId1"/>
@@ -982,9 +982,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1173,67 +1173,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1247,11 +1247,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1502,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1626,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1688,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1750,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1812,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2184,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2246,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2370,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2618,7 +2620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2680,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2742,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2804,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2928,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2990,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3114,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3176,7 +3178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3238,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3300,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3362,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3424,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3486,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3548,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3610,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3672,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3734,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3920,7 +3922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3982,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4106,7 +4108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4168,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4230,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4292,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4354,7 +4356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4416,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4478,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4664,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4726,7 +4728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4788,7 +4790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4912,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4974,7 +4976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5036,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5098,7 +5100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5160,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5222,7 +5224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5284,7 +5286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5346,7 +5348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5408,7 +5410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5470,7 +5472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5532,7 +5534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5594,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5656,142 +5658,142 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5805,13 +5807,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5938,7 +5940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6062,7 +6064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6124,7 +6126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -6186,7 +6188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6248,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6310,7 +6312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6372,7 +6374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6434,7 +6436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6496,7 +6498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6558,7 +6560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6620,7 +6622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6682,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6744,7 +6746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6806,7 +6808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6868,7 +6870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6930,7 +6932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6992,7 +6994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -7054,7 +7056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -7116,7 +7118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -7178,7 +7180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7240,7 +7242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7302,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7364,7 +7366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -7426,7 +7428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -7488,7 +7490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -7550,7 +7552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -7612,7 +7614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -7674,7 +7676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -7736,7 +7738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -7798,7 +7800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -7860,7 +7862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -7922,7 +7924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -7984,7 +7986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8046,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -8108,7 +8110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -8170,7 +8172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -8232,7 +8234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -8294,7 +8296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -8356,7 +8358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -8418,7 +8420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -8480,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -8542,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -8604,7 +8606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -8666,7 +8668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -8728,7 +8730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -8790,7 +8792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -8852,7 +8854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -8914,7 +8916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -8976,7 +8978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -9038,7 +9040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -9100,7 +9102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -9162,7 +9164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -9224,7 +9226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -9286,7 +9288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -9348,7 +9350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -9410,7 +9412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -9472,7 +9474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -9534,7 +9536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -9596,7 +9598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -9658,7 +9660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -9720,7 +9722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -9782,7 +9784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -9844,7 +9846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -9906,7 +9908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -9968,7 +9970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -9991,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68">
         <v>1</v>
@@ -10030,7 +10032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -10092,7 +10094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -10154,7 +10156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -10216,7 +10218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -10278,7 +10280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -10340,7 +10342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -10402,7 +10404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -10464,207 +10466,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -10680,9 +10682,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10744,7 +10746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -10809,7 +10811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10871,487 +10873,487 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -11369,9 +11371,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11433,7 +11435,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -11498,7 +11500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11560,7 +11562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -11622,7 +11624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -11684,7 +11686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -11746,7 +11748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -11808,7 +11810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -11870,7 +11872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -11932,447 +11934,447 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -12386,16 +12388,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12457,7 +12459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -12522,7 +12524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -12584,7 +12586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -12646,7 +12648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -12708,7 +12710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -12770,7 +12772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -12793,7 +12795,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -12832,7 +12834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -12894,7 +12896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -12956,532 +12958,532 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -13495,16 +13497,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.9296875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13566,7 +13568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -13631,7 +13633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -13693,7 +13695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -13755,7 +13757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -13817,7 +13819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -13879,7 +13881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -13941,7 +13943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -14003,7 +14005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -14065,7 +14067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -14127,7 +14129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -14189,7 +14191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -14251,7 +14253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -14313,512 +14315,512 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>

</xml_diff>